<commit_message>
ATULIZAÇÃO DE ERROS DE ENTRADA E SAIDA
</commit_message>
<xml_diff>
--- a/Base de dados/CADASTRO.xlsx
+++ b/Base de dados/CADASTRO.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G308"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -7627,7 +7627,78 @@
       <c r="F308" t="n">
         <v>2</v>
       </c>
-      <c r="G308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>1308</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>TESTE 2</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>RH</t>
+        </is>
+      </c>
+      <c r="D309" s="9" t="n">
+        <v>45721</v>
+      </c>
+      <c r="E309" t="n">
+        <v>2</v>
+      </c>
+      <c r="F309" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>1309</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>TETES 3</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>RH</t>
+        </is>
+      </c>
+      <c r="D310" s="9" t="n">
+        <v>45721</v>
+      </c>
+      <c r="E310" t="n">
+        <v>2</v>
+      </c>
+      <c r="F310" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>1310</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>RH</t>
+        </is>
+      </c>
+      <c r="D311" s="9" t="n">
+        <v>45721</v>
+      </c>
+      <c r="E311" t="n">
+        <v>2</v>
+      </c>
+      <c r="F311" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>